<commit_message>
Wrong index on nitrogen in ARG
</commit_message>
<xml_diff>
--- a/FFparameters.xlsx
+++ b/FFparameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\propertyfit\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="90">
   <si>
     <t>RESNAME</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>OD2</t>
+  </si>
+  <si>
+    <t>NH</t>
   </si>
 </sst>
 </file>
@@ -610,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I435"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,7 +1470,7 @@
         <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>89</v>
       </c>
       <c r="C30">
         <v>-0.84527156702600004</v>
@@ -1496,7 +1499,7 @@
         <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>89</v>
       </c>
       <c r="C31">
         <v>-0.84527156702600004</v>

</xml_diff>